<commit_message>
Yang Li is trying to add his name again as the previous attempt seems not working.
</commit_message>
<xml_diff>
--- a/GitTest.xlsx
+++ b/GitTest.xlsx
@@ -1,10 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9302"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="110" windowWidth="14810" windowHeight="8010"/>
+    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="4">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
   <si>
     <t>Name</t>
   </si>
@@ -26,18 +26,33 @@
   </si>
   <si>
     <t>Yes</t>
+  </si>
+  <si>
+    <t>Yang Li</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Yes</t>
+    <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="Calibri"/>
+      <name val="宋体"/>
       <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="9"/>
+      <name val="宋体"/>
+      <family val="3"/>
+      <charset val="134"/>
       <scheme val="minor"/>
     </font>
   </fonts>
@@ -65,7 +80,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="常规" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleMedium9"/>
@@ -81,7 +96,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 主题​​">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -123,7 +138,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
+        <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -158,7 +173,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -367,15 +382,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B2"/>
+  <dimension ref="A1:B3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+      <selection activeCell="A4" sqref="A4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -383,7 +398,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A2" t="s">
         <v>2</v>
       </c>
@@ -391,7 +406,17 @@
         <v>3</v>
       </c>
     </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A3" t="s">
+        <v>4</v>
+      </c>
+      <c r="B3" t="s">
+        <v>5</v>
+      </c>
+    </row>
   </sheetData>
+  <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>